<commit_message>
developed a linear regression model
</commit_message>
<xml_diff>
--- a/data/news_data/dataset_with_sentiment.xlsx
+++ b/data/news_data/dataset_with_sentiment.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -468,11 +468,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Americans aren't spending like they used to</t>
+          <t>Forget FAANG and GAMMA, the 'Magnificent 7' tech stocks - including Tesla and Nvidia - now dominate the market</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.36</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="3">
@@ -508,11 +508,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>US stocks rise as traders digest upbeat economic data</t>
+          <t>Apple is a great company – but not much is driving the tech giant toward a $3 trillion valuation, analyst says</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.5</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -528,11 +528,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Forget FAANG and GAMMA, the 'Magnificent 7' tech stocks - including Tesla and Nvidia - now dominate the market</t>
+          <t>US stocks rise as traders digest upbeat economic data</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.68</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6">
@@ -548,11 +548,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Apple is a great company – but not much is driving the tech giant toward a $3 trillion valuation, analyst says</t>
+          <t>Americans aren't spending like they used to</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="7">
@@ -568,11 +568,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>A new tech bull market is here - and expect strong second-quarter earnings to add more fuel to the rally, Wedbush analyst Dan Ives says</t>
+          <t>US stocks jump to close strong 2nd quarter as Nasdaq has best first half in decades</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.76</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="8">
@@ -588,11 +588,11 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Get ready for years of terrible stock-market returns as 2 key tailwinds fade, Fed economist warns</t>
+          <t>US stocks rally as inflation cools further, heading for strong 2nd-quarter gains</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.38</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="9">
@@ -608,11 +608,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>US stocks jump to close strong 2nd quarter as Nasdaq has best first half in decades</t>
+          <t>A new tech bull market is here - and expect strong second-quarter earnings to add more fuel to the rally, Wedbush analyst Dan Ives says</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.91</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="10">
@@ -628,11 +628,11 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>US stocks rally as inflation cools further, heading for strong 2nd-quarter gains</t>
+          <t>Stop worrying about a recession - but it's still time to dump overvalued Big Tech stocks, Citi strategist says</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.85</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="11">
@@ -648,11 +648,11 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Stop worrying about a recession - but it's still time to dump overvalued Big Tech stocks, Citi strategist says</t>
+          <t>Get ready for years of terrible stock-market returns as 2 key tailwinds fade, Fed economist warns</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.12</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="12">
@@ -728,11 +728,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Here's why Wall Street's biggest bull thinks the stock market is headed to record highs this year</t>
+          <t>Tesla's record deliveries in Q2 were driven by price cuts and are already priced into its stock, short seller Jim Chanos says</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="16">
@@ -768,11 +768,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Wharton's Jeremy Siegel says the bull run in stocks can go a lot longer even as the Fed wages 'war on growth'</t>
+          <t>Zimbabwe's stock market is up 800% this year as investors seek shelter from blistering 176% inflation rate</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.34</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18">
@@ -808,11 +808,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Tesla's record deliveries in Q2 were driven by price cuts and are already priced into its stock, short seller Jim Chanos says</t>
+          <t>Here's why Wall Street's biggest bull thinks the stock market is headed to record highs this year</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.35</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20">
@@ -828,11 +828,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Tech stock investors are positioned for a 'win-win' outcome regardless of recession risk, Wharton's Jeremy Siegel says</t>
+          <t>Wharton's Jeremy Siegel says the bull run in stocks can go a lot longer even as the Fed wages 'war on growth'</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.2</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="21">
@@ -848,11 +848,11 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Zimbabwe's stock market is up 800% this year as investors seek shelter from blistering 176% inflation rate</t>
+          <t>Tech stock investors are positioned for a 'win-win' outcome regardless of recession risk, Wharton's Jeremy Siegel says</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="22">
@@ -888,11 +888,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>A Sriracha shortage has boosted the cost of a single bottle to $70. It's cheaper to buy a share of Coca-Cola, PayPal, or Pfizer.</t>
+          <t>The 'superbubble' in stocks and housing will burst - but the AI boom might delay the crash, Jeremy Grantham says</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.7</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="24">
@@ -908,11 +908,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>The 'superbubble' in stocks and housing will burst - but the AI boom might delay the crash, Jeremy Grantham says</t>
+          <t>A Sriracha shortage has boosted the cost of a single bottle to $70. It's cheaper to buy a share of Coca-Cola, PayPal, or Pfizer.</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.12</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="25">
@@ -928,11 +928,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>The 'Rule of 10' can help investors identify the next big stock market winners, according to Goldman Sachs</t>
+          <t>US stocks slip as investors await Fed minutes and parse China growth data</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.85</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="26">
@@ -948,11 +948,11 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>US stocks slip as investors await Fed minutes and parse China growth data</t>
+          <t>US stocks slide as Fed minutes show more rate hikes may be on the way</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.73</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="27">
@@ -968,11 +968,11 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>US stocks slide as Fed minutes show more rate hikes may be on the way</t>
+          <t>Netflix's password-sharing crackdown is going so well that one Wall Street bear just upgraded the stock</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.5</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="28">
@@ -988,11 +988,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Netflix's password-sharing crackdown is going so well that one Wall Street bear just upgraded the stock</t>
+          <t>The 'Rule of 10' can help investors identify the next big stock market winners, according to Goldman Sachs</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.71</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="29">
@@ -1008,7 +1008,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>US stocks fall as private payroll data suggests more Fed rate hikes are coming</t>
+          <t>The bull market in stocks is on track to push the S&amp;P 500 to 5,000 by 2024, Bank of America says</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1028,11 +1028,11 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Dow falls more than 300 points as investors brace for more Fed tightening after huge ADP report</t>
+          <t>Why the latest job-market data is a worst-case scenario for stock bulls</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.66</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="31">
@@ -1048,11 +1048,11 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>The bull market in stocks is on track to push the S&amp;P 500 to 5,000 by 2024, Bank of America says</t>
+          <t>Dow falls more than 300 points as investors brace for more Fed tightening after huge ADP report</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.5</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="32">
@@ -1068,11 +1068,11 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>'Big Short' investor Michael Burry predicted inflation would plunge - but his calls of a stock-market crash and recession are yet to come true</t>
+          <t>US stocks fall as private payroll data suggests more Fed rate hikes are coming</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.23</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="33">
@@ -1098,7 +1098,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2023-07-06</t>
+          <t>2023-07-07</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1108,11 +1108,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Why the latest job-market data is a worst-case scenario for stock bulls</t>
+          <t>The US stock rally has no fundamentals and Fed rate hikes will 'break the back' of something in markets, top economist David Rosenberg says</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="35">
@@ -1168,17 +1168,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>The US stock rally has no fundamentals and Fed rate hikes will 'break the back' of something in markets, top economist David Rosenberg says</t>
+          <t>SVB, BBBY, Lordstown lead list of US bankruptcies as companies fold up at the fastest pace since 2010</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2023-07-07</t>
+          <t>2023-07-09</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1188,17 +1188,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>SVB, BBBY, Lordstown lead list of US bankruptcies as companies fold up at the fastest pace since 2010</t>
+          <t>The AI boom has boosted the 'Magnificent 7' stocks' combined market cap to $11 trillion - that's nearly triple Germany's GDP.</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.5</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2023-07-09</t>
+          <t>2023-07-10</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1208,11 +1208,11 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>The AI boom has boosted the 'Magnificent 7' stocks' combined market cap to $11 trillion - that's nearly triple Germany's GDP.</t>
+          <t>Even Wall Street has no clue which way the economy is going</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.88</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="40">
@@ -1238,7 +1238,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2023-07-10</t>
+          <t>2023-07-11</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1248,11 +1248,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Even Wall Street has no clue which way the economy is going</t>
+          <t>AI has to show it's like the internet in 1995 – not the Metaverse in 2021</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.35</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="42">
@@ -1288,17 +1288,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>AI has to show it's like the internet in 1995 – not the Metaverse in 2021</t>
+          <t>What tech boom? A homebuilder, 3 cruise lines, and Chipotle have all outperformed Apple and Microsoft on the S&amp;P 500 this year</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.68</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2023-07-11</t>
+          <t>2023-07-12</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1308,11 +1308,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>What tech boom? A homebuilder, 3 cruise lines, and Chipotle have all outperformed Apple and Microsoft on the S&amp;P 500 this year</t>
+          <t>US stocks climb as traders hope cooler June inflation means end to Fed tightening</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.5</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="45">
@@ -1328,11 +1328,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>US stocks climb as traders hope cooler June inflation means end to Fed tightening</t>
+          <t>Why the lowest inflation reading in 2 years is great news for the stock market</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.72</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="46">
@@ -1348,11 +1348,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>US stocks jump as investors cheer lowest inflation reading in over 2 years</t>
+          <t>Here's where history says the latest bull market is headed next</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.59</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="47">
@@ -1368,11 +1368,11 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>The economy is in a 'rolling financial crisis' as private sector debt balloons, GMO says</t>
+          <t>US stocks jump as investors cheer lowest inflation reading in over 2 years</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.12</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="48">
@@ -1388,17 +1388,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Why the lowest inflation reading in 2 years is great news for the stock market</t>
+          <t>The economy is in a 'rolling financial crisis' as private sector debt balloons, GMO says</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.68</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2023-07-12</t>
+          <t>2023-07-13</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1408,11 +1408,11 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Here's where history says the latest bull market is headed next</t>
+          <t>US stocks climb as more signs of cooling inflation lift hopes that Fed rate hikes are near an end</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.5</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="50">
@@ -1428,7 +1428,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>US stocks climb as more signs of cooling inflation lift hopes that Fed rate hikes are near an end</t>
+          <t>Stocks are headed to new records as inflation is crumbling and Fed can breathe easier, Fundstrat's Tom Lee says</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1438,7 +1438,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2023-07-13</t>
+          <t>2023-07-14</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1448,11 +1448,11 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Stocks are headed to new records as inflation is crumbling and Fed can breathe easier, Fundstrat's Tom Lee says</t>
+          <t>Hedge funds are reeling from some of the worst outflows since the Great Recession and managers are shunning Wall Street – even as a bull market reigns</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.71</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="52">
@@ -1468,11 +1468,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>US stocks rise after banks set positive tone for 2nd-quarter earnings</t>
+          <t>US stocks trade mixed but notch a weekly gain as earnings impress and inflation cools</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.78</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="53">
@@ -1488,11 +1488,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Hedge funds are reeling from some of the worst outflows since the Great Recession and managers are shunning Wall Street – even as a bull market reigns</t>
+          <t>US stocks rise after banks set positive tone for 2nd-quarter earnings</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.29</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="54">
@@ -1508,11 +1508,11 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>US stocks trade mixed but notch a weekly gain as earnings impress and inflation cools</t>
+          <t>Investors are once again chasing some of the most speculative names in the stock market</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.93</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="55">
@@ -1528,17 +1528,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Investors are once again chasing some of the most speculative names in the stock market</t>
+          <t>'I don't see why people are going to sell their stocks.' 'Big Short' investor Steve Eisman says stocks will keep rallying as long as the economy stays healthy</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.59</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2023-07-14</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1548,17 +1548,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>'I don't see why people are going to sell their stocks.' 'Big Short' investor Steve Eisman says stocks will keep rallying as long as the economy stays healthy</t>
+          <t>Here are 5 questions investors should consider when jumping into the huge rally in the 'Magnificent 7' stocks this year</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0.7</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2023-07-16</t>
+          <t>2023-07-17</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1568,11 +1568,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Here are 5 questions investors should consider when jumping into the huge rally in the 'Magnificent 7' stocks this year</t>
+          <t>US stocks trade mixed as China's GDP growth disappoints and investors brace for big week of earnings</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.87</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="58">
@@ -1588,11 +1588,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>US stocks rally as recession fears ease and investors look to upcoming Big Tech earnings</t>
+          <t>Elite investor Seth Klarman warns the 'everything bubble' might still burst - and more banking disasters may be coming</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>0.26</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="59">
@@ -1608,11 +1608,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>US stocks trade mixed as China's GDP growth disappoints and investors brace for big week of earnings</t>
+          <t>Stocks could get slammed by a rebound in inflation and weak corporate earnings, Wells Fargo wealth management CIO says</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0.5</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="60">
@@ -1648,17 +1648,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Stocks could get slammed by a rebound in inflation and weak corporate earnings, Wells Fargo wealth management CIO says</t>
+          <t>US stocks rally as recession fears ease and investors look to upcoming Big Tech earnings</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0.66</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2023-07-17</t>
+          <t>2023-07-18</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1668,11 +1668,11 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Elite investor Seth Klarman warns the 'everything bubble' might still burst - and more banking disasters may be coming</t>
+          <t>US stocks dip as retail sales miss forecasts while earnings season ramps up</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.18</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="63">
@@ -1688,11 +1688,11 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>US stocks dip as retail sales miss forecasts while earnings season ramps up</t>
+          <t>Dow extends winning streak to 7 days as US stocks jump on strong bank earnings</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>0.42</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="64">
@@ -1708,11 +1708,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Microsoft adds $154 billion in market value after it announces $30 per month AI subscription</t>
+          <t>The first ETF offering protection against 100% of stock losses just launched</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0.67</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="65">
@@ -1748,17 +1748,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>The first ETF offering protection against 100% of stock losses just launched</t>
+          <t>Microsoft adds $154 billion in market value after it announces $30 per month AI subscription</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>0.35</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2023-07-18</t>
+          <t>2023-07-19</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1768,11 +1768,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Dow extends winning streak to 7 days as US stocks jump on strong bank earnings</t>
+          <t>Microsoft's market value soared as much as $154 billion in just a day. That nearly matched Jeff Bezos' entire fortune.</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0.9</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="68">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>A secretive US asset manager bet big on Tesla in 2011 after a young analyst saw its potential. The stock is up nearly 15,000% since then.</t>
+          <t>Dow hits 8-day winning streak as investors hope for more upbeat earnings reports</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0.68</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="69">
@@ -1808,11 +1808,11 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Dow hits 8-day winning streak as investors hope for more upbeat earnings reports</t>
+          <t>These 4 bearish scenarios could rock the stock market by the end of the year</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0.87</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="70">
@@ -1828,11 +1828,11 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Microsoft's market value soared as much as $154 billion in just a day. That nearly matched Jeff Bezos' entire fortune.</t>
+          <t>Investors pumped $45 billion into stocks last month, the biggest inflow in over a year as recession fears melt away</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.67</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="71">
@@ -1848,11 +1848,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Apple just added $71 billion in market value on news it's developing an 'Apple GPT' AI</t>
+          <t>A secretive US asset manager bet big on Tesla in 2011 after a young analyst saw its potential. The stock is up nearly 15,000% since then.</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="72">
@@ -1868,17 +1868,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>These 4 bearish scenarios could rock the stock market by the end of the year</t>
+          <t>Apple just added $71 billion in market value on news it's developing an 'Apple GPT' AI</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.5</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2023-07-19</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -1888,11 +1888,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Investors pumped $45 billion into stocks last month, the biggest inflow in over a year as recession fears melt away</t>
+          <t>'Something very strange' explains why a US recession has been delayed</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="74">
@@ -1908,11 +1908,11 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>A top economist says the stock-market mania reminds him of the dot-com and housing bubbles - and warns consumers are feeling the squeeze</t>
+          <t>Stock market strategist raises S&amp;P 500 price target by 16% to 4,700 as rally keeps defying skeptics</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0.61</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="75">
@@ -1928,11 +1928,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>'Something very strange' explains why a US recession has been delayed</t>
+          <t>A top economist says the stock-market mania reminds him of the dot-com and housing bubbles - and warns consumers are feeling the squeeze</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>0.15</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="76">
@@ -1948,11 +1948,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Dow eyes 9-day win streak as US stocks trade mixed after Tesla, Netflix earnings</t>
+          <t>This 'gamechanger' technology is harder than rocket science and will drive the next AI wave, Goldman Sachs says</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0.79</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="77">
@@ -1968,17 +1968,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Stock market strategist raises S&amp;P 500 price target by 16% to 4,700 as rally keeps defying skeptics</t>
+          <t>Dow eyes 9-day win streak as US stocks trade mixed after Tesla, Netflix earnings</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0.45</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2023-07-20</t>
+          <t>2023-07-21</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>This 'gamechanger' technology is harder than rocket science and will drive the next AI wave, Goldman Sachs says</t>
+          <t>US stocks trade mixed as Dow caps off its longest winning streak since 2017</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0.5</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="79">
@@ -2008,11 +2008,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>US stocks trade mixed as Dow caps off its longest winning streak since 2017</t>
+          <t>'Shark Tank' investor Kevin O'Leary says Bidenomics has been fantastic for the S&amp;P 500 but bad for small businesses</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.76</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="80">
@@ -2028,17 +2028,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>'Shark Tank' investor Kevin O'Leary says Bidenomics has been fantastic for the S&amp;P 500 but bad for small businesses</t>
+          <t>US stocks rise with Dow heading for 10-day streak of gains as traders sift through earnings</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>0.23</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2023-07-21</t>
+          <t>2023-07-22</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2048,11 +2048,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>US stocks rise with Dow heading for 10-day streak of gains as traders sift through earnings</t>
+          <t>Why 'Barbenheimer' might not be enough to fuel a movie stock rally</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0.67</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="82">
@@ -2078,7 +2078,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2023-07-22</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2088,11 +2088,11 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Why 'Barbenheimer' might not be enough to fuel a movie stock rally</t>
+          <t>The S&amp;P 500 is moving on from its Big Tech fixation, but that could mean smaller 3rd-quarter gains</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>0.5</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="84">
@@ -2108,11 +2108,11 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>A more than 100-year-old buy signal just flashed in the stock market</t>
+          <t>US stocks have rallied so hard that the market is setting its sights on all-time highs once again</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>0.5</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="85">
@@ -2128,11 +2128,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>The S&amp;P 500 is moving on from its Big Tech fixation, but that could mean smaller 3rd-quarter gains</t>
+          <t>Xi Jinping's politburo is set to weigh up how to revive China's faltering economy</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0.74</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="86">
@@ -2168,17 +2168,17 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>US stocks have rallied so hard that the market is setting its sights on all-time highs once again</t>
+          <t>A more than 100-year-old buy signal just flashed in the stock market</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>0.39</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2023-07-24</t>
+          <t>2023-07-25</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2188,11 +2188,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Xi Jinping's politburo is set to weigh up how to revive China's faltering economy</t>
+          <t>A long-time market bear who called the 2000 and 2008 crashes warns the S&amp;P 500 could plummet 64%, bursting a historic bubble</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>0.67</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="89">
@@ -2208,11 +2208,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>The US is headed for a roaring economic boom, thanks to AI, robots, quantum computers, market veteran Ed Yardeni says</t>
+          <t>JPMorgan stays bearish on the stock market and warns that an AI bubble is brewing amid record concentration in mega-cap stocks</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>0.72</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="90">
@@ -2228,17 +2228,17 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>JPMorgan stays bearish on the stock market and warns that an AI bubble is brewing amid record concentration in mega-cap stocks</t>
+          <t>The US is headed for a roaring economic boom, thanks to AI, robots, quantum computers, market veteran Ed Yardeni says</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>0.45</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2023-07-25</t>
+          <t>2023-07-26</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2248,17 +2248,17 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>A long-time market bear who called the 2000 and 2008 crashes warns the S&amp;P 500 could plummet 64%, bursting a historic bubble</t>
+          <t>Traders are betting against American Airlines and Ralph Lauren with a recession still on the table</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>0.45</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2023-07-25</t>
+          <t>2023-07-26</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -2268,11 +2268,11 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>US stocks trade mixed as the Fed begins its 2-day policy meeting</t>
+          <t>The US stock market has become a 'get-rich-quick' scheme that's ignoring oncoming economic pain, top economist David Rosenberg says</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>0.5</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="93">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>The US stock market has become a 'get-rich-quick' scheme that's ignoring oncoming economic pain, top economist David Rosenberg says</t>
+          <t>The Dow's win streak is at risk as US stocks drop ahead of expected Fed rate hike</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>0.18</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="94">
@@ -2308,17 +2308,17 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Traders are betting against American Airlines and Ralph Lauren with a recession still on the table</t>
+          <t>There are 5 reasons why earnings will continue to defy expectations and fuel the stock-market rally, State Street says</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>0.29</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2023-07-26</t>
+          <t>2023-07-27</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2328,17 +2328,17 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>There are 5 reasons why earnings will continue to defy expectations and fuel the stock-market rally, State Street says</t>
+          <t>Jerome Powell fielded a question about 'Barbie' and Taylor Swift in a snooze of a Fed meeting</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2023-07-26</t>
+          <t>2023-07-27</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2348,11 +2348,11 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>The Dow's win streak is at risk as US stocks drop ahead of expected Fed rate hike</t>
+          <t>US stocks climb as the Dow heads for longest winning streak in 126 years</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>0.58</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="97">
@@ -2368,17 +2368,17 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>US stocks climb as the Dow heads for longest winning streak in 126 years</t>
+          <t>Dow snaps historic win streak as US stocks fall amid more earnings results</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2023-07-27</t>
+          <t>2023-07-28</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2388,17 +2388,17 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Dow snaps historic win streak as US stocks fall amid more earnings results</t>
+          <t>The extreme bubble in stocks 'will end in tears' with the S&amp;P 500 plunging 64%, a long-time bear who called the 2000, 2008 crashes has warned. Here are his 6 best quotes.</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>0.79</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2023-07-27</t>
+          <t>2023-07-28</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2408,17 +2408,17 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Jerome Powell fielded a question about 'Barbie' and Taylor Swift in a snooze of a Fed meeting</t>
+          <t>Dow and S&amp;P 500 finish 3rd straight winning week as more data shows inflation is cooling</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>0.6</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2023-07-28</t>
+          <t>2023-07-29</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2428,17 +2428,17 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>The Dow's rally is broadening as first-half laggards catch up</t>
+          <t>The Dow's latest winning streak is bad news for stocks - and a recession might be underway, top economist David Rosenberg says</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2023-07-28</t>
+          <t>2023-07-29</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2448,11 +2448,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>The extreme bubble in stocks 'will end in tears' with the S&amp;P 500 plunging 64%, a long-time bear who called the 2000, 2008 crashes has warned. Here are his 6 best quotes.</t>
+          <t>The Fed's newfound focus on data is bad news for the sliding dollar</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>0.65</v>
+        <v>0.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>